<commit_message>
finalized motif and cleavage tables
</commit_message>
<xml_diff>
--- a/genome_annotation_and_characterization/conserved_motifs.xlsx
+++ b/genome_annotation_and_characterization/conserved_motifs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gwenddolenkettenburg/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BA91CC-6B9E-1F4A-82F0-3A88D9563DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75624C8-DB91-9846-A44E-DF971232FB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="13500" windowHeight="17260" xr2:uid="{2350210B-B243-1547-BD80-B8D2E8F7443A}"/>
+    <workbookView xWindow="240" yWindow="740" windowWidth="20460" windowHeight="17300" xr2:uid="{2350210B-B243-1547-BD80-B8D2E8F7443A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="397">
   <si>
     <t>mischivirus</t>
   </si>
@@ -1086,6 +1086,147 @@
   </si>
   <si>
     <t>G(1950)WS</t>
+  </si>
+  <si>
+    <t>MN784123</t>
+  </si>
+  <si>
+    <t>mandrill</t>
+  </si>
+  <si>
+    <t>JN867757</t>
+  </si>
+  <si>
+    <t>HF677705</t>
+  </si>
+  <si>
+    <t>shellfish</t>
+  </si>
+  <si>
+    <t>OM105025</t>
+  </si>
+  <si>
+    <t>NC_033776</t>
+  </si>
+  <si>
+    <t>G(1226)KPGAGKS</t>
+  </si>
+  <si>
+    <t>G(1550)RPGAGKS</t>
+  </si>
+  <si>
+    <t>G(1706)MCG</t>
+  </si>
+  <si>
+    <t>K(1918)DEIR</t>
+  </si>
+  <si>
+    <t>G(2018)MCG</t>
+  </si>
+  <si>
+    <t>Y(2090)GDD</t>
+  </si>
+  <si>
+    <t>F(2137)LKR</t>
+  </si>
+  <si>
+    <t>K(2230)DEIR</t>
+  </si>
+  <si>
+    <t>Y(2402)GDD</t>
+  </si>
+  <si>
+    <t>F(2449)LKR</t>
+  </si>
+  <si>
+    <t>S(1474)EPGQGKS</t>
+  </si>
+  <si>
+    <t>G(1972)MCG</t>
+  </si>
+  <si>
+    <t>K(2181)DELR</t>
+  </si>
+  <si>
+    <t>Y(2347)GDD</t>
+  </si>
+  <si>
+    <t>F(2395)LKR</t>
+  </si>
+  <si>
+    <t>JX437642*</t>
+  </si>
+  <si>
+    <t>A(280)GPGPVKS</t>
+  </si>
+  <si>
+    <t>G(335)AFG</t>
+  </si>
+  <si>
+    <t>G(462)PPGIGKT</t>
+  </si>
+  <si>
+    <t>G(478)IPGIGKT</t>
+  </si>
+  <si>
+    <t>K(934)GKNK</t>
+  </si>
+  <si>
+    <t>K(945)GKTK</t>
+  </si>
+  <si>
+    <t>D(951)DEYDE</t>
+  </si>
+  <si>
+    <t>D(960)DEYEE</t>
+  </si>
+  <si>
+    <t>G(1159)DCG</t>
+  </si>
+  <si>
+    <t>G(1168)DCG</t>
+  </si>
+  <si>
+    <t>W(1203)KGL</t>
+  </si>
+  <si>
+    <t>W(1213)KGL</t>
+  </si>
+  <si>
+    <t>K(1263)DELR</t>
+  </si>
+  <si>
+    <t>K(1375)DELR</t>
+  </si>
+  <si>
+    <t>D(1438)YSKWDST</t>
+  </si>
+  <si>
+    <t>D(1450)YSKWDST</t>
+  </si>
+  <si>
+    <t>G(1493)LPSG</t>
+  </si>
+  <si>
+    <t>G(1505)LPSG</t>
+  </si>
+  <si>
+    <t>Y(1541)GDD</t>
+  </si>
+  <si>
+    <t>Y(1553)GDD</t>
+  </si>
+  <si>
+    <t>P(1836)PG</t>
+  </si>
+  <si>
+    <t>P(1849)PG</t>
+  </si>
+  <si>
+    <t>G(1980)WS</t>
+  </si>
+  <si>
+    <t>G(1995)WS</t>
   </si>
 </sst>
 </file>
@@ -1452,10 +1593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31531B08-202E-D840-BAC2-584C47BCD981}">
-  <dimension ref="A2:M78"/>
+  <dimension ref="A2:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1463,9 +1604,9 @@
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.6640625" bestFit="1" customWidth="1"/>
@@ -1575,290 +1716,287 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>205</v>
-      </c>
-      <c r="E8" t="s">
-        <v>206</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" t="s">
-        <v>91</v>
-      </c>
-      <c r="H9" t="s">
-        <v>96</v>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>351</v>
+      </c>
+      <c r="B6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" t="s">
+        <v>358</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
+        <v>361</v>
+      </c>
+      <c r="F6" t="s">
+        <v>364</v>
+      </c>
+      <c r="G6" t="s">
+        <v>365</v>
+      </c>
+      <c r="H6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>359</v>
+      </c>
+      <c r="F7" t="s">
+        <v>360</v>
+      </c>
+      <c r="G7" t="s">
+        <v>362</v>
+      </c>
+      <c r="H7" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
+        <v>206</v>
       </c>
       <c r="F10" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>62</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>85</v>
       </c>
-      <c r="D11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" t="s">
         <v>87</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F13" t="s">
         <v>89</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G13" t="s">
         <v>92</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>353</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>205</v>
+        <v>367</v>
       </c>
       <c r="E14" t="s">
-        <v>206</v>
+        <v>368</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>369</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>370</v>
       </c>
       <c r="H14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" t="s">
-        <v>132</v>
-      </c>
-      <c r="F15" t="s">
-        <v>99</v>
-      </c>
-      <c r="G15" t="s">
-        <v>100</v>
-      </c>
-      <c r="H15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>105</v>
-      </c>
-      <c r="D16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" t="s">
-        <v>133</v>
-      </c>
-      <c r="F16" t="s">
-        <v>106</v>
-      </c>
-      <c r="G16" t="s">
-        <v>107</v>
-      </c>
-      <c r="H16" t="s">
-        <v>108</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>206</v>
       </c>
       <c r="F17" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
       <c r="H17" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
         <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="F18" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="H18" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>61</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D19" t="s">
         <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="G19" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="H19" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>61</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D20" t="s">
         <v>81</v>
       </c>
       <c r="E20" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="F20" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="H20" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1866,132 +2004,132 @@
         <v>63</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D21" t="s">
         <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="G21" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="H21" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="2"/>
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" t="s">
+        <v>120</v>
+      </c>
+      <c r="G22" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" t="s">
+        <v>126</v>
+      </c>
+      <c r="H23" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>205</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>206</v>
+        <v>128</v>
       </c>
       <c r="F24" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="H24" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" t="s">
-        <v>135</v>
-      </c>
-      <c r="D25" t="s">
-        <v>223</v>
-      </c>
-      <c r="E25" t="s">
-        <v>136</v>
-      </c>
-      <c r="F25" t="s">
-        <v>137</v>
-      </c>
-      <c r="G25" t="s">
-        <v>138</v>
-      </c>
-      <c r="H25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>140</v>
-      </c>
-      <c r="D26" t="s">
-        <v>224</v>
-      </c>
-      <c r="E26" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" t="s">
-        <v>142</v>
-      </c>
-      <c r="G26" t="s">
-        <v>143</v>
-      </c>
-      <c r="H26" t="s">
-        <v>144</v>
-      </c>
+      <c r="B25" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>145</v>
+        <v>205</v>
       </c>
       <c r="E27" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="F27" t="s">
-        <v>147</v>
+        <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="H27" t="s">
-        <v>149</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1999,25 +2137,25 @@
         <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>150</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>223</v>
       </c>
       <c r="E28" t="s">
-        <v>81</v>
+        <v>136</v>
       </c>
       <c r="F28" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="G28" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="H28" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -2025,25 +2163,25 @@
         <v>61</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>151</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
       <c r="D29" t="s">
-        <v>81</v>
+        <v>224</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>141</v>
       </c>
       <c r="F29" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="G29" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="H29" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -2051,218 +2189,218 @@
         <v>61</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="E30" t="s">
-        <v>154</v>
+        <v>225</v>
       </c>
       <c r="F30" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G30" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="H30" t="s">
-        <v>81</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>32</v>
+      <c r="B31" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="C31" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D31" t="s">
-        <v>226</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>227</v>
+        <v>81</v>
       </c>
       <c r="F31" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
       <c r="G31" t="s">
-        <v>158</v>
+        <v>81</v>
       </c>
       <c r="H31" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>46</v>
+        <v>61</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="C32" t="s">
-        <v>161</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>160</v>
+        <v>81</v>
       </c>
       <c r="E32" t="s">
-        <v>229</v>
+        <v>81</v>
       </c>
       <c r="F32" t="s">
-        <v>162</v>
+        <v>81</v>
       </c>
       <c r="G32" t="s">
-        <v>163</v>
+        <v>81</v>
       </c>
       <c r="H32" t="s">
-        <v>164</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" t="s">
+        <v>154</v>
+      </c>
+      <c r="F33" t="s">
+        <v>155</v>
+      </c>
+      <c r="G33" t="s">
+        <v>81</v>
+      </c>
+      <c r="H33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" t="s">
+        <v>226</v>
+      </c>
+      <c r="E34" t="s">
+        <v>227</v>
+      </c>
+      <c r="F34" t="s">
+        <v>157</v>
+      </c>
+      <c r="G34" t="s">
+        <v>158</v>
+      </c>
+      <c r="H34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" t="s">
-        <v>165</v>
-      </c>
-      <c r="D33" t="s">
-        <v>228</v>
-      </c>
-      <c r="E33" t="s">
-        <v>230</v>
-      </c>
-      <c r="F33" t="s">
-        <v>166</v>
-      </c>
-      <c r="G33" t="s">
-        <v>167</v>
-      </c>
-      <c r="H33" t="s">
-        <v>168</v>
+      <c r="B35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
+        <v>161</v>
+      </c>
+      <c r="D35" t="s">
+        <v>160</v>
+      </c>
+      <c r="E35" t="s">
+        <v>229</v>
+      </c>
+      <c r="F35" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35" t="s">
+        <v>163</v>
+      </c>
+      <c r="H35" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" t="s">
-        <v>12</v>
+        <v>63</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="D36" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="E36" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
+        <v>166</v>
       </c>
       <c r="G36" t="s">
-        <v>23</v>
+        <v>167</v>
       </c>
       <c r="H36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" t="s">
-        <v>169</v>
-      </c>
-      <c r="D37" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" t="s">
-        <v>183</v>
-      </c>
-      <c r="F37" t="s">
-        <v>170</v>
-      </c>
-      <c r="G37" t="s">
-        <v>171</v>
-      </c>
-      <c r="H37" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" t="s">
-        <v>173</v>
-      </c>
-      <c r="D38" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" t="s">
-        <v>184</v>
-      </c>
-      <c r="F38" t="s">
-        <v>174</v>
-      </c>
-      <c r="G38" t="s">
-        <v>175</v>
-      </c>
-      <c r="H38" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>48</v>
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
       <c r="E39" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="F39" t="s">
-        <v>179</v>
+        <v>22</v>
       </c>
       <c r="G39" t="s">
-        <v>180</v>
+        <v>23</v>
       </c>
       <c r="H39" t="s">
-        <v>181</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D40" t="s">
         <v>81</v>
@@ -2282,756 +2420,696 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C41" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D41" t="s">
         <v>81</v>
       </c>
       <c r="E41" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F41" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G41" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="H41" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D42" t="s">
         <v>81</v>
       </c>
       <c r="E42" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F42" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="G42" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H42" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="2"/>
+      <c r="A43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" t="s">
+        <v>182</v>
+      </c>
+      <c r="D43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" t="s">
+        <v>183</v>
+      </c>
+      <c r="F43" t="s">
+        <v>170</v>
+      </c>
+      <c r="G43" t="s">
+        <v>171</v>
+      </c>
+      <c r="H43" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" t="s">
+        <v>182</v>
+      </c>
+      <c r="D44" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" t="s">
+        <v>183</v>
+      </c>
+      <c r="F44" t="s">
+        <v>170</v>
+      </c>
+      <c r="G44" t="s">
+        <v>171</v>
+      </c>
+      <c r="H44" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" t="s">
-        <v>14</v>
+        <v>66</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>21</v>
+        <v>185</v>
       </c>
       <c r="D45" t="s">
-        <v>205</v>
+        <v>81</v>
       </c>
       <c r="E45" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="F45" t="s">
-        <v>22</v>
+        <v>187</v>
       </c>
       <c r="G45" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="H45" t="s">
-        <v>24</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" t="s">
-        <v>190</v>
-      </c>
-      <c r="D46" t="s">
-        <v>208</v>
-      </c>
-      <c r="E46" t="s">
-        <v>207</v>
-      </c>
-      <c r="F46" t="s">
-        <v>191</v>
-      </c>
-      <c r="G46" t="s">
-        <v>192</v>
-      </c>
-      <c r="H46" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" t="s">
-        <v>194</v>
-      </c>
-      <c r="D47" t="s">
-        <v>193</v>
-      </c>
-      <c r="E47" t="s">
-        <v>209</v>
-      </c>
-      <c r="F47" t="s">
-        <v>195</v>
-      </c>
-      <c r="G47" t="s">
-        <v>196</v>
-      </c>
-      <c r="H47" t="s">
-        <v>197</v>
-      </c>
+      <c r="B46" s="2"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>198</v>
+        <v>60</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>199</v>
+        <v>21</v>
       </c>
       <c r="D48" t="s">
-        <v>81</v>
+        <v>205</v>
+      </c>
+      <c r="E48" t="s">
+        <v>206</v>
       </c>
       <c r="F48" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="G48" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="H48" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>61</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>34</v>
+      <c r="B49" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D49" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="E49" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F49" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="G49" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="H49" t="s">
-        <v>204</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>61</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>52</v>
+      <c r="B50" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C50" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="D50" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="E50" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F50" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="G50" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="H50" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>61</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>53</v>
+      <c r="B51" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="C51" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="D51" t="s">
-        <v>217</v>
-      </c>
-      <c r="E51" t="s">
-        <v>219</v>
+        <v>81</v>
       </c>
       <c r="F51" t="s">
-        <v>220</v>
+        <v>81</v>
       </c>
       <c r="G51" t="s">
-        <v>221</v>
+        <v>81</v>
       </c>
       <c r="H51" t="s">
-        <v>222</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" t="s">
+        <v>201</v>
+      </c>
+      <c r="D52" t="s">
+        <v>200</v>
+      </c>
+      <c r="E52" t="s">
+        <v>210</v>
+      </c>
+      <c r="F52" t="s">
+        <v>202</v>
+      </c>
+      <c r="G52" t="s">
+        <v>203</v>
+      </c>
+      <c r="H52" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" t="s">
+        <v>212</v>
+      </c>
+      <c r="D53" t="s">
+        <v>211</v>
+      </c>
+      <c r="E53" t="s">
+        <v>213</v>
+      </c>
+      <c r="F53" t="s">
+        <v>214</v>
+      </c>
+      <c r="G53" t="s">
+        <v>215</v>
+      </c>
+      <c r="H53" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" t="s">
-        <v>17</v>
+        <v>61</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>21</v>
+        <v>218</v>
       </c>
       <c r="D54" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="E54" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="F54" t="s">
-        <v>22</v>
+        <v>220</v>
       </c>
       <c r="G54" t="s">
-        <v>23</v>
+        <v>221</v>
       </c>
       <c r="H54" t="s">
-        <v>24</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>61</v>
-      </c>
-      <c r="B55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C55" t="s">
+        <v>373</v>
+      </c>
+      <c r="D55" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" t="s">
+        <v>374</v>
+      </c>
+      <c r="F55" t="s">
+        <v>81</v>
+      </c>
+      <c r="G55" t="s">
+        <v>81</v>
+      </c>
+      <c r="H55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" t="s">
+        <v>205</v>
+      </c>
+      <c r="E58" t="s">
+        <v>206</v>
+      </c>
+      <c r="F58" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58" t="s">
+        <v>23</v>
+      </c>
+      <c r="H58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C59" t="s">
         <v>231</v>
       </c>
-      <c r="D55" t="s">
-        <v>81</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="D59" t="s">
+        <v>81</v>
+      </c>
+      <c r="E59" t="s">
         <v>232</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F59" t="s">
         <v>233</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G59" t="s">
         <v>234</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H59" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C56" t="s">
-        <v>236</v>
-      </c>
-      <c r="D56" t="s">
-        <v>81</v>
-      </c>
-      <c r="E56" t="s">
-        <v>244</v>
-      </c>
-      <c r="F56" t="s">
-        <v>245</v>
-      </c>
-      <c r="G56" t="s">
-        <v>246</v>
-      </c>
-      <c r="H56" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>61</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C57" t="s">
-        <v>247</v>
-      </c>
-      <c r="D57" t="s">
-        <v>81</v>
-      </c>
-      <c r="E57" t="s">
-        <v>248</v>
-      </c>
-      <c r="F57" t="s">
-        <v>249</v>
-      </c>
-      <c r="G57" t="s">
-        <v>250</v>
-      </c>
-      <c r="H57" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" t="s">
-        <v>18</v>
+        <v>61</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="C60" t="s">
-        <v>21</v>
+        <v>236</v>
       </c>
       <c r="D60" t="s">
-        <v>205</v>
+        <v>81</v>
       </c>
       <c r="E60" t="s">
-        <v>206</v>
+        <v>244</v>
       </c>
       <c r="F60" t="s">
-        <v>22</v>
+        <v>245</v>
       </c>
       <c r="G60" t="s">
-        <v>23</v>
+        <v>246</v>
       </c>
       <c r="H60" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>239</v>
+      <c r="B61" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C61" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D61" t="s">
         <v>81</v>
       </c>
       <c r="E61" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F61" t="s">
-        <v>81</v>
+        <v>249</v>
       </c>
       <c r="G61" t="s">
-        <v>81</v>
+        <v>250</v>
       </c>
       <c r="H61" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C62" t="s">
-        <v>254</v>
-      </c>
-      <c r="D62" t="s">
-        <v>81</v>
-      </c>
-      <c r="E62" t="s">
-        <v>255</v>
-      </c>
-      <c r="F62" t="s">
-        <v>256</v>
-      </c>
-      <c r="G62" t="s">
-        <v>257</v>
-      </c>
-      <c r="H62" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C63" t="s">
-        <v>259</v>
-      </c>
-      <c r="D63" t="s">
-        <v>81</v>
-      </c>
-      <c r="E63" t="s">
-        <v>260</v>
-      </c>
-      <c r="F63" t="s">
-        <v>261</v>
-      </c>
-      <c r="G63" t="s">
-        <v>111</v>
-      </c>
-      <c r="H63" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
       </c>
       <c r="C64" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="D64" t="s">
-        <v>81</v>
+        <v>205</v>
       </c>
       <c r="E64" t="s">
-        <v>264</v>
+        <v>206</v>
       </c>
       <c r="F64" t="s">
-        <v>265</v>
+        <v>22</v>
       </c>
       <c r="G64" t="s">
-        <v>266</v>
+        <v>23</v>
       </c>
       <c r="H64" t="s">
-        <v>267</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>56</v>
+      <c r="B65" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="C65" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="D65" t="s">
         <v>81</v>
       </c>
       <c r="E65" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="F65" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G65" t="s">
-        <v>270</v>
+        <v>81</v>
       </c>
       <c r="H65" t="s">
-        <v>271</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C66" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="D66" t="s">
         <v>81</v>
       </c>
       <c r="E66" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="F66" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="G66" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="H66" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C67" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="D67" t="s">
         <v>81</v>
       </c>
       <c r="E67" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="F67" t="s">
-        <v>90</v>
+        <v>261</v>
       </c>
       <c r="G67" t="s">
-        <v>279</v>
+        <v>111</v>
       </c>
       <c r="H67" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B68" s="2"/>
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C68" t="s">
+        <v>263</v>
+      </c>
+      <c r="D68" t="s">
+        <v>81</v>
+      </c>
+      <c r="E68" t="s">
+        <v>264</v>
+      </c>
+      <c r="F68" t="s">
+        <v>265</v>
+      </c>
+      <c r="G68" t="s">
+        <v>266</v>
+      </c>
+      <c r="H68" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>61</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C69" t="s">
+        <v>268</v>
+      </c>
+      <c r="D69" t="s">
+        <v>81</v>
+      </c>
+      <c r="E69" t="s">
+        <v>269</v>
+      </c>
+      <c r="F69" t="s">
+        <v>88</v>
+      </c>
+      <c r="G69" t="s">
+        <v>270</v>
+      </c>
+      <c r="H69" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>60</v>
-      </c>
-      <c r="B70" t="s">
-        <v>19</v>
+        <v>66</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C70" t="s">
-        <v>38</v>
+        <v>272</v>
       </c>
       <c r="D70" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="E70" t="s">
-        <v>40</v>
+        <v>273</v>
       </c>
       <c r="F70" t="s">
-        <v>25</v>
+        <v>274</v>
       </c>
       <c r="G70" t="s">
-        <v>41</v>
+        <v>275</v>
       </c>
       <c r="H70" t="s">
-        <v>22</v>
-      </c>
-      <c r="I70" t="s">
-        <v>287</v>
-      </c>
-      <c r="J70" t="s">
-        <v>42</v>
-      </c>
-      <c r="K70" t="s">
-        <v>23</v>
-      </c>
-      <c r="L70" t="s">
-        <v>298</v>
-      </c>
-      <c r="M70" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>61</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>20</v>
+      <c r="B71" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C71" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D71" t="s">
-        <v>282</v>
+        <v>81</v>
       </c>
       <c r="E71" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F71" t="s">
-        <v>284</v>
+        <v>90</v>
       </c>
       <c r="G71" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="H71" t="s">
-        <v>286</v>
-      </c>
-      <c r="I71" t="s">
-        <v>288</v>
-      </c>
-      <c r="J71" t="s">
-        <v>289</v>
-      </c>
-      <c r="K71" t="s">
-        <v>290</v>
-      </c>
-      <c r="L71" t="s">
-        <v>291</v>
-      </c>
-      <c r="M71" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>61</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C72" t="s">
-        <v>293</v>
-      </c>
-      <c r="D72" t="s">
-        <v>294</v>
-      </c>
-      <c r="E72" t="s">
-        <v>295</v>
-      </c>
-      <c r="F72" t="s">
-        <v>296</v>
-      </c>
-      <c r="G72" t="s">
-        <v>297</v>
-      </c>
-      <c r="H72" t="s">
-        <v>81</v>
-      </c>
-      <c r="I72" t="s">
-        <v>81</v>
-      </c>
-      <c r="J72" t="s">
-        <v>81</v>
-      </c>
-      <c r="K72" t="s">
-        <v>81</v>
-      </c>
-      <c r="L72" t="s">
-        <v>81</v>
-      </c>
-      <c r="M72" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>61</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C73" t="s">
-        <v>81</v>
-      </c>
-      <c r="D73" t="s">
-        <v>81</v>
-      </c>
-      <c r="E73" t="s">
-        <v>81</v>
-      </c>
-      <c r="F73" t="s">
-        <v>81</v>
-      </c>
-      <c r="G73" t="s">
-        <v>81</v>
-      </c>
-      <c r="H73" t="s">
-        <v>81</v>
-      </c>
-      <c r="I73" t="s">
-        <v>81</v>
-      </c>
-      <c r="J73" t="s">
-        <v>81</v>
-      </c>
-      <c r="K73" t="s">
-        <v>81</v>
-      </c>
-      <c r="L73" t="s">
-        <v>300</v>
-      </c>
-      <c r="M73" t="s">
-        <v>301</v>
-      </c>
+      <c r="B72" s="2"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>61</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>242</v>
+        <v>60</v>
+      </c>
+      <c r="B74" t="s">
+        <v>19</v>
       </c>
       <c r="C74" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="D74" t="s">
-        <v>302</v>
+        <v>39</v>
       </c>
       <c r="E74" t="s">
-        <v>303</v>
+        <v>40</v>
       </c>
       <c r="F74" t="s">
-        <v>304</v>
+        <v>25</v>
       </c>
       <c r="G74" t="s">
-        <v>305</v>
+        <v>41</v>
       </c>
       <c r="H74" t="s">
-        <v>306</v>
+        <v>22</v>
       </c>
       <c r="I74" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="J74" t="s">
-        <v>308</v>
+        <v>42</v>
       </c>
       <c r="K74" t="s">
-        <v>317</v>
+        <v>23</v>
       </c>
       <c r="L74" t="s">
-        <v>81</v>
+        <v>298</v>
       </c>
       <c r="M74" t="s">
-        <v>81</v>
+        <v>299</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
@@ -3039,163 +3117,409 @@
         <v>61</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>243</v>
+        <v>20</v>
       </c>
       <c r="C75" t="s">
-        <v>81</v>
+        <v>281</v>
       </c>
       <c r="D75" t="s">
-        <v>309</v>
+        <v>282</v>
       </c>
       <c r="E75" t="s">
-        <v>310</v>
+        <v>283</v>
       </c>
       <c r="F75" t="s">
-        <v>311</v>
+        <v>284</v>
       </c>
       <c r="G75" t="s">
-        <v>312</v>
+        <v>285</v>
       </c>
       <c r="H75" t="s">
-        <v>313</v>
+        <v>286</v>
       </c>
       <c r="I75" t="s">
-        <v>314</v>
+        <v>288</v>
       </c>
       <c r="J75" t="s">
-        <v>315</v>
+        <v>289</v>
       </c>
       <c r="K75" t="s">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="L75" t="s">
-        <v>81</v>
+        <v>291</v>
       </c>
       <c r="M75" t="s">
-        <v>81</v>
+        <v>292</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>61</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>44</v>
+      <c r="B76" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="C76" t="s">
-        <v>318</v>
+        <v>293</v>
       </c>
       <c r="D76" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
       <c r="E76" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="F76" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="G76" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="H76" t="s">
-        <v>322</v>
+        <v>81</v>
       </c>
       <c r="I76" t="s">
-        <v>323</v>
+        <v>81</v>
       </c>
       <c r="J76" t="s">
-        <v>324</v>
+        <v>81</v>
       </c>
       <c r="K76" t="s">
-        <v>325</v>
+        <v>81</v>
       </c>
       <c r="L76" t="s">
-        <v>326</v>
+        <v>81</v>
       </c>
       <c r="M76" t="s">
-        <v>327</v>
+        <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>61</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>37</v>
+      <c r="B77" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="C77" t="s">
-        <v>328</v>
+        <v>81</v>
       </c>
       <c r="D77" t="s">
-        <v>329</v>
+        <v>81</v>
       </c>
       <c r="E77" t="s">
-        <v>330</v>
+        <v>81</v>
       </c>
       <c r="F77" t="s">
-        <v>331</v>
+        <v>81</v>
       </c>
       <c r="G77" t="s">
-        <v>332</v>
+        <v>81</v>
       </c>
       <c r="H77" t="s">
-        <v>333</v>
+        <v>81</v>
       </c>
       <c r="I77" t="s">
-        <v>334</v>
+        <v>81</v>
       </c>
       <c r="J77" t="s">
-        <v>335</v>
+        <v>81</v>
       </c>
       <c r="K77" t="s">
-        <v>336</v>
+        <v>81</v>
       </c>
       <c r="L77" t="s">
-        <v>337</v>
+        <v>300</v>
       </c>
       <c r="M77" t="s">
-        <v>338</v>
+        <v>301</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>61</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C78" t="s">
+        <v>81</v>
+      </c>
+      <c r="D78" t="s">
+        <v>302</v>
+      </c>
+      <c r="E78" t="s">
+        <v>303</v>
+      </c>
+      <c r="F78" t="s">
+        <v>304</v>
+      </c>
+      <c r="G78" t="s">
+        <v>305</v>
+      </c>
+      <c r="H78" t="s">
+        <v>306</v>
+      </c>
+      <c r="I78" t="s">
+        <v>307</v>
+      </c>
+      <c r="J78" t="s">
+        <v>308</v>
+      </c>
+      <c r="K78" t="s">
+        <v>317</v>
+      </c>
+      <c r="L78" t="s">
+        <v>81</v>
+      </c>
+      <c r="M78" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>61</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C79" t="s">
+        <v>81</v>
+      </c>
+      <c r="D79" t="s">
+        <v>309</v>
+      </c>
+      <c r="E79" t="s">
+        <v>310</v>
+      </c>
+      <c r="F79" t="s">
+        <v>311</v>
+      </c>
+      <c r="G79" t="s">
+        <v>312</v>
+      </c>
+      <c r="H79" t="s">
+        <v>313</v>
+      </c>
+      <c r="I79" t="s">
+        <v>314</v>
+      </c>
+      <c r="J79" t="s">
+        <v>315</v>
+      </c>
+      <c r="K79" t="s">
+        <v>316</v>
+      </c>
+      <c r="L79" t="s">
+        <v>81</v>
+      </c>
+      <c r="M79" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>61</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C80" t="s">
+        <v>318</v>
+      </c>
+      <c r="D80" t="s">
+        <v>319</v>
+      </c>
+      <c r="E80" t="s">
+        <v>309</v>
+      </c>
+      <c r="F80" t="s">
+        <v>320</v>
+      </c>
+      <c r="G80" t="s">
+        <v>321</v>
+      </c>
+      <c r="H80" t="s">
+        <v>322</v>
+      </c>
+      <c r="I80" t="s">
+        <v>323</v>
+      </c>
+      <c r="J80" t="s">
+        <v>324</v>
+      </c>
+      <c r="K80" t="s">
+        <v>325</v>
+      </c>
+      <c r="L80" t="s">
+        <v>326</v>
+      </c>
+      <c r="M80" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>61</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C81" t="s">
+        <v>328</v>
+      </c>
+      <c r="D81" t="s">
+        <v>329</v>
+      </c>
+      <c r="E81" t="s">
+        <v>330</v>
+      </c>
+      <c r="F81" t="s">
+        <v>331</v>
+      </c>
+      <c r="G81" t="s">
+        <v>332</v>
+      </c>
+      <c r="H81" t="s">
+        <v>333</v>
+      </c>
+      <c r="I81" t="s">
+        <v>334</v>
+      </c>
+      <c r="J81" t="s">
+        <v>335</v>
+      </c>
+      <c r="K81" t="s">
+        <v>336</v>
+      </c>
+      <c r="L81" t="s">
+        <v>337</v>
+      </c>
+      <c r="M81" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>66</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C82" t="s">
         <v>339</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D82" t="s">
         <v>340</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E82" t="s">
         <v>341</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F82" t="s">
         <v>342</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G82" t="s">
         <v>343</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H82" t="s">
         <v>344</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I82" t="s">
         <v>345</v>
       </c>
-      <c r="J78" t="s">
+      <c r="J82" t="s">
         <v>346</v>
       </c>
-      <c r="K78" t="s">
+      <c r="K82" t="s">
         <v>347</v>
       </c>
-      <c r="L78" t="s">
+      <c r="L82" t="s">
         <v>348</v>
       </c>
-      <c r="M78" t="s">
+      <c r="M82" t="s">
         <v>349</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>354</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C83" t="s">
+        <v>375</v>
+      </c>
+      <c r="D83" t="s">
+        <v>377</v>
+      </c>
+      <c r="E83" t="s">
+        <v>379</v>
+      </c>
+      <c r="F83" t="s">
+        <v>381</v>
+      </c>
+      <c r="G83" t="s">
+        <v>383</v>
+      </c>
+      <c r="H83" t="s">
+        <v>385</v>
+      </c>
+      <c r="I83" t="s">
+        <v>387</v>
+      </c>
+      <c r="J83" t="s">
+        <v>389</v>
+      </c>
+      <c r="K83" t="s">
+        <v>391</v>
+      </c>
+      <c r="L83" t="s">
+        <v>393</v>
+      </c>
+      <c r="M83" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>61</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C84" t="s">
+        <v>376</v>
+      </c>
+      <c r="D84" t="s">
+        <v>378</v>
+      </c>
+      <c r="E84" t="s">
+        <v>380</v>
+      </c>
+      <c r="F84" t="s">
+        <v>382</v>
+      </c>
+      <c r="G84" t="s">
+        <v>384</v>
+      </c>
+      <c r="H84" t="s">
+        <v>386</v>
+      </c>
+      <c r="I84" t="s">
+        <v>388</v>
+      </c>
+      <c r="J84" t="s">
+        <v>390</v>
+      </c>
+      <c r="K84" t="s">
+        <v>392</v>
+      </c>
+      <c r="L84" t="s">
+        <v>394</v>
+      </c>
+      <c r="M84" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>